<commit_message>
finished downloads of 5-flag system representatives
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/2023-07-16_add.xlsx
+++ b/flag/AQB_classification/2023-07-16_add.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/bioinfRhints/flag/AQB_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B673895D-55F2-8140-9016-FE8C7EB75629}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5EECD8-7D80-254D-81E2-41430D7E2486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14620" yWindow="500" windowWidth="36200" windowHeight="23120" activeTab="2" xr2:uid="{FBB23AE7-A21D-2740-9EDC-4927A339D3B1}"/>
+    <workbookView xWindow="14600" yWindow="500" windowWidth="36200" windowHeight="23120" activeTab="2" xr2:uid="{FBB23AE7-A21D-2740-9EDC-4927A339D3B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
1214 seqs, including AQB classification ie Ferreira&Beeby, Liu Ochman, powerSource identified
</commit_message>
<xml_diff>
--- a/flag/AQB_classification/2023-07-16_add.xlsx
+++ b/flag/AQB_classification/2023-07-16_add.xlsx
@@ -1,44 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nickm/GitHub/bioinfRhints/flag/AQB_classification/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nmat471/HD/GitHub/bioinfRhints/flag/AQB_classification/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD5EECD8-7D80-254D-81E2-41430D7E2486}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18F73878-67BC-3B4B-9973-40BE9191E739}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14600" yWindow="500" windowWidth="36200" windowHeight="23120" activeTab="2" xr2:uid="{FBB23AE7-A21D-2740-9EDC-4927A339D3B1}"/>
+    <workbookView xWindow="14120" yWindow="500" windowWidth="36200" windowHeight="23120" activeTab="2" xr2:uid="{FBB23AE7-A21D-2740-9EDC-4927A339D3B1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="merge" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="642">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2150" uniqueCount="643">
   <si>
     <t>Species used in Figures 1B and C</t>
   </si>
@@ -1964,6 +1953,9 @@
   </si>
   <si>
     <t>covered by V583</t>
+  </si>
+  <si>
+    <t>suppressed</t>
   </si>
 </sst>
 </file>
@@ -1994,12 +1986,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2014,7 +2012,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2030,6 +2028,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4840,7 +4839,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="P3:Q680">
+  <sortState ref="P3:Q680">
     <sortCondition ref="P3:P680"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5132,8 +5131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B9D5D3D-DF78-3F49-A41C-226229F9925D}">
   <dimension ref="A1:U291"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A239" workbookViewId="0">
-      <selection activeCell="G249" sqref="G249"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E81" sqref="E81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6025,13 +6024,14 @@
       <c r="D31" t="s">
         <v>274</v>
       </c>
-      <c r="E31" t="s">
+      <c r="E31" s="7" t="s">
         <v>429</v>
       </c>
-      <c r="G31" t="s">
+      <c r="F31" s="7"/>
+      <c r="G31" s="7" t="s">
         <v>257</v>
       </c>
-      <c r="H31" t="s">
+      <c r="H31" s="7" t="s">
         <v>216</v>
       </c>
       <c r="I31" t="s">
@@ -11724,12 +11724,15 @@
       <c r="E291" t="s">
         <v>640</v>
       </c>
+      <c r="G291" t="s">
+        <v>642</v>
+      </c>
       <c r="H291" t="s">
         <v>637</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U288">
+  <sortState ref="A2:U288">
     <sortCondition ref="E2:E288"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>